<commit_message>
Ajuste del caso de prueba CP_LOGIN_001 en el archivo login
</commit_message>
<xml_diff>
--- a/docs/test-cases/login.xlsx
+++ b/docs/test-cases/login.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C82F2-6803-42F9-A369-D71004A946A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -202,8 +203,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -296,9 +297,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -587,14 +585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="3" width="16.85546875" customWidth="1"/>
@@ -609,7 +607,7 @@
     <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42" customHeight="1">
+    <row r="1" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="150">
+    <row r="2" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -685,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -719,7 +717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="57">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -753,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -787,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -821,33 +819,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="105.75" customHeight="1">
+    <row r="7" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="3" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
se agrega caso de prueba CP_LOGIN_002
</commit_message>
<xml_diff>
--- a/docs/test-cases/login.xlsx
+++ b/docs/test-cases/login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C82F2-6803-42F9-A369-D71004A946A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBCD10E-66C0-4A71-8349-9D434089502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,7 +589,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se comenta código de captura de errores
</commit_message>
<xml_diff>
--- a/docs/test-cases/login.xlsx
+++ b/docs/test-cases/login.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBCD10E-66C0-4A71-8349-9D434089502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -203,8 +202,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,14 +584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="3" width="16.85546875" customWidth="1"/>
@@ -607,7 +606,7 @@
     <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="42" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="102.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -683,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -717,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="57">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -751,7 +750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -785,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="75">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -819,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="105.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>

</xml_diff>